<commit_message>
fixed the all_games data
</commit_message>
<xml_diff>
--- a/all_games.xlsx
+++ b/all_games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evankim/Desktop/Projects/Water-Polo-Analytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE92C190-1D71-CD40-9B35-A481A9EB22C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DA43F5-6E75-3E42-A67F-061B49CEF33C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2124" uniqueCount="870">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2130" uniqueCount="870">
   <si>
     <t>Number of Passes</t>
   </si>
@@ -2994,8 +2994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="P200" sqref="P200"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4486,6 +4486,9 @@
       <c r="N19">
         <v>1</v>
       </c>
+      <c r="O19" t="s">
+        <v>28</v>
+      </c>
       <c r="P19">
         <v>0</v>
       </c>
@@ -11026,6 +11029,9 @@
       <c r="N97">
         <v>1</v>
       </c>
+      <c r="O97" t="s">
+        <v>28</v>
+      </c>
       <c r="P97">
         <v>0</v>
       </c>
@@ -11423,6 +11429,9 @@
       <c r="N102">
         <v>1</v>
       </c>
+      <c r="O102" t="s">
+        <v>28</v>
+      </c>
       <c r="P102">
         <v>0</v>
       </c>
@@ -11900,6 +11909,9 @@
       <c r="N108" t="s">
         <v>28</v>
       </c>
+      <c r="O108" t="s">
+        <v>28</v>
+      </c>
       <c r="P108">
         <v>0</v>
       </c>
@@ -11977,6 +11989,9 @@
       <c r="N109">
         <v>1</v>
       </c>
+      <c r="O109" t="s">
+        <v>28</v>
+      </c>
       <c r="P109">
         <v>0</v>
       </c>
@@ -12213,6 +12228,9 @@
       </c>
       <c r="N112">
         <v>1</v>
+      </c>
+      <c r="O112" t="s">
+        <v>28</v>
       </c>
       <c r="P112">
         <v>0</v>

</xml_diff>